<commit_message>
tenant owner email done
</commit_message>
<xml_diff>
--- a/output1.xlsx
+++ b/output1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,10 +501,20 @@
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>is_active</t>
+          <t>is_tenant_active</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>is_paid</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>rent_token</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>created</t>
         </is>
@@ -515,43 +525,47 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>169</v>
+        <v>181</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>roopa</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
+          <t>roopa apartment</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>roopamugappa@gmail.com</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>roopa</t>
+          <t>roopa staish</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>lohegoan</t>
+          <t>lohegoan,pune</t>
         </is>
       </c>
       <c r="G2" t="n">
         <v>2</v>
       </c>
       <c r="H2" t="n">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>9538774485</t>
+          <t>8880869502</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>10111</t>
+          <t>10500</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2023-02-26</t>
+          <t>2023-02-15</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -559,14 +573,30 @@
           <t>123412341234</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>/media/adhar_card/DSC03793_HJZNgVo.JPG</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>/media/Propery_image/DSC03794_hcjVbNe.JPG</t>
+        </is>
+      </c>
       <c r="O2" t="b">
         <v>1</v>
       </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>2023-02-24T07:02:02.132311Z</t>
+      <c r="P2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>71617a98-06df-4d89-9d25-2098b88e6d3b</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>2023-02-28T10:12:09.232550Z</t>
         </is>
       </c>
     </row>
@@ -575,70 +605,558 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>179</v>
+        <v>217</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>my app</t>
+          <t>av</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>roopa@gmail.com</t>
+          <t>dk@gmail.com</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>dsjkn</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>lohegoan</t>
+          <t>dnjna</t>
         </is>
       </c>
       <c r="G3" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3" t="n">
+        <v>32</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>0987654321</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>234567</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>2023-03-15</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>098765432112</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>/media/adhar_card/Screenshot_15_ZFVgEyF.png</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>/media/Propery_image/Screenshot_9_rfprr6V.png</t>
+        </is>
+      </c>
+      <c r="O3" t="b">
+        <v>1</v>
+      </c>
+      <c r="P3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>ebf8a454-64f5-4540-b20e-24b0fc9f0941</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>2023-03-01T10:05:31.225030Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="H3" t="n">
+      <c r="B4" t="n">
+        <v>220</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>DragonStone</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>syrax@gmail.com</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Rhaenyra</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>across black water bay</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>10</v>
+      </c>
+      <c r="H4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>1111222233</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>2019-04-11</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>123456789098</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>/media/a/da</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>/media/a/tvdes</t>
+        </is>
+      </c>
+      <c r="O4" t="b">
+        <v>1</v>
+      </c>
+      <c r="P4" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>4b9ecea3-2c61-4542-adc3-5ee461324f8e</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>2023-03-02T06:27:14.830277Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>221</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Sept of Baelor</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>sparrow@gmail.com</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>High Sparrow</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>kingslanding</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>10</v>
+      </c>
+      <c r="H5" t="n">
+        <v>60</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2233221111</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>4000</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>2019-04-11</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>98765432111</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>/media/a/da</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>/media/a/tvdes</t>
+        </is>
+      </c>
+      <c r="O5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>b6bccff5-02c3-472a-ba22-2d16a8efbba4</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>2023-03-02T06:27:14.917219Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>222</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Red Keep</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>queen@gmail.com</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Cersei</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Under the rubble</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
         <v>2</v>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>8880860503</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>100100</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>2023-02-19</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>123412341233</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>/media/adhar_card/DSC03793_j1MtERw.JPG</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>/media/Propery_image/DSC03794_S5OZ2RM.JPG</t>
-        </is>
-      </c>
-      <c r="O3" t="b">
-        <v>1</v>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>2023-02-25T17:57:57.830786Z</t>
+      <c r="H6" t="n">
+        <v>40</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>1111444433</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>2019-04-11</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>123456789099</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>/media/a/da</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>/media/a/tvdes</t>
+        </is>
+      </c>
+      <c r="O6" t="b">
+        <v>1</v>
+      </c>
+      <c r="P6" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>b5ea7a7f-a1fd-42bb-8b43-8f7ff9a3a293</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>2023-03-02T06:27:15.028138Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>223</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Iron Island</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>yara@gmail.com</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">yara </t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>some where in the ocean</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>3</v>
+      </c>
+      <c r="H7" t="n">
+        <v>30</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>3311331100</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>6000</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>2019-04-11</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>123456789000</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>/media/a/da</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>/media/a/tvdes</t>
+        </is>
+      </c>
+      <c r="O7" t="b">
+        <v>1</v>
+      </c>
+      <c r="P7" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>19e31b89-8552-4936-9d54-1d8b8ba0dec7</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>2023-03-02T06:27:15.189049Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>226</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Joel C Varughese</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>joelvarughese257@gmail.com</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Joel C Varughese</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Bharti Nagar, wd 18 , Bargarh</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>2</v>
+      </c>
+      <c r="H8" t="n">
+        <v>22</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>0891730149</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>2023-03-21</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>123456789012</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>/media/adhar_card/Screenshot_43_NGNPzDc.png</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>/media/Propery_image/Screenshot_7_yqlvtOm.png</t>
+        </is>
+      </c>
+      <c r="O8" t="b">
+        <v>1</v>
+      </c>
+      <c r="P8" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>41500cbd-fd52-4f20-a3e0-bb8e90af3af7</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>2023-03-02T09:44:26.725009Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>227</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>ad@gmail.com</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>2</v>
+      </c>
+      <c r="H9" t="n">
+        <v>2</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>1234123412</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>2023-03-21</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>121212121211</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>/media/adhar_card/Screenshot_8_Sa1m7YQ.png</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>/media/Propery_image/Screenshot_8_85aJKrU.png</t>
+        </is>
+      </c>
+      <c r="O9" t="b">
+        <v>1</v>
+      </c>
+      <c r="P9" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>a0b9bb2c-9da0-4b44-9c83-4cc3e3f0b1f5</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>2023-03-02T10:20:22.185042Z</t>
         </is>
       </c>
     </row>

</xml_diff>